<commit_message>
updated Dockerfile to use non-root user
</commit_message>
<xml_diff>
--- a/data/2 Cholera partnership coverage.xlsx
+++ b/data/2 Cholera partnership coverage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef.sharepoint.com/teams/MOZ/Programmes/SHAREPOINT/5. Emergency Response Management/Cholera 2023/1 Partnership/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{B462CD15-D6FC-5741-AA84-E24B6D69E78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{252F9804-6445-B245-8B35-3E9B5FEA950F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{B462CD15-D6FC-5741-AA84-E24B6D69E78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B3275D-9C8D-A042-9AAE-03ED743A6983}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="500" windowWidth="33900" windowHeight="23500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="2" r:id="rId1"/>
@@ -2464,7 +2464,7 @@
   <dimension ref="A1:Y162"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E2" sqref="E2:E162"/>
@@ -2590,7 +2590,7 @@
         <v>53</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>389</v>
+        <v>56</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -2782,7 +2782,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>67</v>
+        <v>389</v>
       </c>
       <c r="V8" s="6">
         <v>1</v>
@@ -3670,7 +3670,7 @@
         <v>257</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>67</v>
+        <v>389</v>
       </c>
       <c r="S53" s="6">
         <v>1</v>
@@ -3753,7 +3753,7 @@
         <v>264</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>389</v>
+        <v>56</v>
       </c>
       <c r="K57" s="6">
         <v>1</v>
@@ -4054,7 +4054,7 @@
         <v>91</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>67</v>
+        <v>389</v>
       </c>
       <c r="V74" s="6">
         <v>1</v>
@@ -4708,7 +4708,7 @@
         <v>278</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>389</v>
+        <v>56</v>
       </c>
       <c r="P101" s="6">
         <v>1</v>
@@ -4833,7 +4833,7 @@
         <v>292</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>67</v>
+        <v>389</v>
       </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
@@ -5156,7 +5156,7 @@
         <v>155</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>389</v>
+        <v>56</v>
       </c>
       <c r="R121" s="6">
         <v>1</v>
@@ -5179,7 +5179,7 @@
         <v>157</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>389</v>
+        <v>56</v>
       </c>
       <c r="H122" s="6">
         <v>1</v>
@@ -6361,6 +6361,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6410,7 +6419,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="MOZ Documents" ma:contentTypeID="0x010100D3D94803219734408FFC4A2CF4F8CC3F000AF5CE343721734C85F7674E37810420" ma:contentTypeVersion="67" ma:contentTypeDescription="MOZ Content Types" ma:contentTypeScope="" ma:versionID="f5ade075a55c831507ec8a4defb6ba92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5" xmlns:ns4="90583e5e-655e-4438-8618-262f6cb9882d" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="209b9c5416e4fe328bc325e7efdaf9db" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6737,7 +6746,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -6771,25 +6780,24 @@
     <l373856d30794c63a26ebe024fcf0a28 xmlns="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </l373856d30794c63a26ebe024fcf0a28>
-    <_dlc_DocId xmlns="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5">MOZA-2122242090-78388</_dlc_DocId>
+    <_dlc_DocId xmlns="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5">MOZA-2122242090-81461</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5">
-      <Url>https://unicef.sharepoint.com/teams/MOZ/Programmes/_layouts/15/DocIdRedir.aspx?ID=MOZA-2122242090-78388</Url>
-      <Description>MOZA-2122242090-78388</Description>
+      <Url>https://unicef.sharepoint.com/teams/MOZ/Programmes/_layouts/15/DocIdRedir.aspx?ID=MOZA-2122242090-81461</Url>
+      <Description>MOZA-2122242090-81461</Description>
     </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73406F81-AA70-44F8-A525-258A87E22992}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74963540-D02A-450B-97C8-C1F8B8B9D8B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -6798,7 +6806,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{827430A4-1E47-417A-90FA-70AED4BE4D7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6821,30 +6829,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4251CF3E-3044-4B26-AD26-5C1C977907BE}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
     <ds:schemaRef ds:uri="90583e5e-655e-4438-8618-262f6cb9882d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9a3b62e3-6f96-49a3-97e4-fe5d09ffedd5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73406F81-AA70-44F8-A525-258A87E22992}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>